<commit_message>
clean all models benchs
</commit_message>
<xml_diff>
--- a/models_data/all_models_plot_set_FULL_results.xlsx
+++ b/models_data/all_models_plot_set_FULL_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -220,9 +220,6 @@
     <t xml:space="preserve">drop</t>
   </si>
   <si>
-    <t xml:space="preserve">Citation</t>
-  </si>
-  <si>
     <t xml:space="preserve">mistralai/mixtral-8x22b-v0.1</t>
   </si>
   <si>
@@ -235,21 +232,12 @@
     <t xml:space="preserve">together_ai/meta-llama/Llama-2-70b-chat-hf</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.databricks.com/blog/introducing-dbrx-new-state-art-open-llm</t>
-  </si>
-  <si>
     <t xml:space="preserve">together_ai/meta-llama/Llama-2-13b-chat-hf</t>
   </si>
   <si>
-    <t xml:space="preserve">https://arxiv.org/abs/2307.09289</t>
-  </si>
-  <si>
     <t xml:space="preserve">together_ai/meta-llama/Llama-2-7b-chat-hf</t>
   </si>
   <si>
-    <t xml:space="preserve">https://arxiv.org/abs/2307.09290</t>
-  </si>
-  <si>
     <t xml:space="preserve">together_ai/meta-llama/Llama-3-70b-chat-hf</t>
   </si>
   <si>
@@ -286,9 +274,6 @@
     <t xml:space="preserve">claude-3-opus-20240229</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www-cdn.anthropic.com/de8ba9b01c9ab7cbabf5c33b80b7bbc618857627/Model_Card_Claude_3.pdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">claude-3-sonnet-20240229</t>
   </si>
   <si>
@@ -301,16 +286,10 @@
     <t xml:space="preserve">gpt-4-0613</t>
   </si>
   <si>
-    <t xml:space="preserve">https://arxiv.org/pdf/2303.08774</t>
-  </si>
-  <si>
     <t xml:space="preserve">gpt-3.5-turbo-0125</t>
   </si>
   <si>
     <t xml:space="preserve">gemini/gemini-pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://arxiv.org/pdf/2312.11805</t>
   </si>
   <si>
     <t xml:space="preserve">Mistral-large-2402</t>
@@ -370,6 +349,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -634,18 +614,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BO30"/>
+  <dimension ref="A1:BN30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BR18" activeCellId="0" sqref="BR18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -844,13 +825,10 @@
       <c r="BN1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="3" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>0.667235494880546</v>
@@ -1042,9 +1020,9 @@
         <v>0.777949965322547</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>0.631399317406143</v>
@@ -1236,9 +1214,9 @@
         <v>0.718154365546603</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>0.568259385665529</v>
@@ -1426,7 +1404,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BJ5" s="3" t="n">
         <v>0.805051302288871</v>
@@ -1439,14 +1417,11 @@
       </c>
       <c r="BM5" s="3" t="n">
         <v>0.639</v>
-      </c>
-      <c r="BO5" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="BJ6" s="3" t="n">
         <v>0.745067087608524</v>
@@ -1459,14 +1434,11 @@
       </c>
       <c r="BM6" s="3" t="n">
         <v>0.658</v>
-      </c>
-      <c r="BO6" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="BJ7" s="3" t="n">
         <v>0.717442778216259</v>
@@ -1480,13 +1452,10 @@
       <c r="BM7" s="3" t="n">
         <v>0.548</v>
       </c>
-      <c r="BO7" s="3" t="s">
-        <v>75</v>
-      </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>0.681740614334471</v>
@@ -1678,9 +1647,9 @@
         <v>0.800592231799543</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>0.571672354948805</v>
@@ -1872,9 +1841,9 @@
         <v>0.670721995784583</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>0.660409556313993</v>
@@ -2066,9 +2035,9 @@
         <v>0.757282461670731</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>0.477815699658703</v>
@@ -2260,9 +2229,9 @@
         <v>0.535170310018511</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>0.404436860068259</v>
@@ -2454,9 +2423,9 @@
         <v>0.376481868282916</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>0.651877133105802</v>
@@ -2648,9 +2617,9 @@
         <v>0.774609194640082</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>0.629692832764505</v>
@@ -2842,9 +2811,9 @@
         <v>0.749931323079671</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>0.545221843003413</v>
@@ -3036,9 +3005,9 @@
         <v>0.685154096374267</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>0.523037542662116</v>
@@ -3230,9 +3199,9 @@
         <v>0.616476685490625</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>0.404436860068259</v>
@@ -3424,9 +3393,9 @@
         <v>0.555546251226632</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3" t="n">
         <v>0.366894197952218</v>
@@ -3620,7 +3589,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3" t="n">
         <v>0.964</v>
@@ -3630,14 +3599,11 @@
       </c>
       <c r="BM19" s="3" t="n">
         <v>0.868</v>
-      </c>
-      <c r="BO19" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3" t="n">
         <v>0.932</v>
@@ -3647,14 +3613,11 @@
       </c>
       <c r="BM20" s="3" t="n">
         <v>0.79</v>
-      </c>
-      <c r="BO20" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B21" s="3" t="n">
         <v>0.892</v>
@@ -3665,13 +3628,10 @@
       <c r="BM21" s="3" t="n">
         <v>0.752</v>
       </c>
-      <c r="BO21" s="3" t="s">
-        <v>88</v>
-      </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="BM22" s="3" t="n">
         <v>0.8048</v>
@@ -3679,7 +3639,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B23" s="3" t="n">
         <v>0.963</v>
@@ -3690,13 +3650,10 @@
       <c r="BM23" s="3" t="n">
         <v>0.864</v>
       </c>
-      <c r="BO23" s="3" t="s">
-        <v>93</v>
-      </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B24" s="3" t="n">
         <v>0.852</v>
@@ -3707,18 +3664,15 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="BM25" s="3" t="n">
         <v>0.718</v>
       </c>
-      <c r="BO25" s="3" t="s">
-        <v>96</v>
-      </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B26" s="3" t="n">
         <v>0.914</v>
@@ -3730,25 +3684,25 @@
         <v>0.812</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="BM27" s="3" t="n">
         <v>0.722</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="BM28" s="3" t="n">
         <v>0.796</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="BM29" s="3" t="n">
         <v>0.887</v>
@@ -3756,19 +3710,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="BM30" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="BM30" s="1" t="n">
         <v>0.737</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="BO5" r:id="rId1" display="https://www.databricks.com/blog/introducing-dbrx-new-state-art-open-llm"/>
-    <hyperlink ref="BO19" r:id="rId2" display="https://www-cdn.anthropic.com/de8ba9b01c9ab7cbabf5c33b80b7bbc618857627/Model_Card_Claude_3.pdf"/>
-    <hyperlink ref="BO20" r:id="rId3" display="https://www-cdn.anthropic.com/de8ba9b01c9ab7cbabf5c33b80b7bbc618857627/Model_Card_Claude_3.pdf"/>
-    <hyperlink ref="BO21" r:id="rId4" display="https://www-cdn.anthropic.com/de8ba9b01c9ab7cbabf5c33b80b7bbc618857627/Model_Card_Claude_3.pdf"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>